<commit_message>
arquivo certo - pcp - gestão
</commit_message>
<xml_diff>
--- a/6SEM/AGO005-Gestão de Projetos/JINDER/Plano de Comunicação do Projeto - JINDER.xlsx
+++ b/6SEM/AGO005-Gestão de Projetos/JINDER/Plano de Comunicação do Projeto - JINDER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fernanda Reis\fatec\6SEM\AGO005-Gestão de Projetos\JINDER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E581B068-95AD-4D71-A0D6-0A5159D07B73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8995DD02-3FA4-46F8-9E6A-057808E86C20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ECFD472F-0084-4C82-B139-A372E69F4568}"/>
   </bookViews>
@@ -301,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -313,26 +313,30 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -648,10 +652,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B05B51-0F98-408B-A4E0-6AB10AB98C70}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -669,18 +676,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="24.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
@@ -696,323 +703,323 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="F3" s="11" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="F3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="7"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="13"/>
     </row>
     <row r="7" spans="1:10" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:10" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="J8" s="7"/>
+      <c r="J8" s="13"/>
     </row>
     <row r="9" spans="1:10" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="11" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="6" t="s">
+      <c r="I11" s="13"/>
+      <c r="J11" s="11" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
     </row>
     <row r="13" spans="1:10" ht="114" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="I13" s="12"/>
-      <c r="J13" s="6" t="s">
+      <c r="I13" s="15"/>
+      <c r="J13" s="11" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="7"/>
+      <c r="B19" s="6"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="7"/>
+      <c r="B20" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1021,6 +1028,6 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="59" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>